<commit_message>
Course Duration & troubleshooting LO detail
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,42 +365,52 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>version_number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>course_duration</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>course_summary</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>course_objective</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>learning_objective_detail</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>course_type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>skill_level</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>site_link</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>lead_developer</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>course_reviewer</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>learning_objective_detail</t>
         </is>
       </c>
     </row>
@@ -410,44 +420,52 @@
           <t>Advanced Natural Language Processing in Python</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>6 Hours</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>This course will focus on four key topics in Natural Language Processing: information retrieval, classification, sentiment analysis and topic modelling. Information retrieval covers the building blocks of a search engine - the inverted index and maps out in detail with both illustrations and code how an information retrieval application can be built. Three disparate, classical approaches will be examined to fulfil this objective. Classification will then be outlined, focusing on its supervised machine learning foundations. A real-world classification problem of news classification will be illustrated using a BBC news dataset. Classification will again be enacted to undertake sentiment analysis. Key challanges in the field of sentiment analysis will also be explored.  Topic Modelling as the name suggests is a process to automatically identify topics present in a datset. The course will demostrate from a practical perspective how this can be attained.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Participants should attain specialist knowledge and skills to enable development of more challenging language based applications like sentiment analysis and search engines.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Describe the boolean retrieval model; Execute the boolean retrieval model over a dataset; Describe the vector space model; Execute the vector space model over a dataset.; Describe how a language model can be used to enact retrieval over a dataset; Execute a language modelling approach to enact retrieval over a dataset; Describe supervised machine learning; Describe pathway of a typical machine learning project; Follow steps in pathway to enact classification over a dataset; Describe sentiment analysis; Describe challenges in a sentiment analysis task; Execute sentiment analysis using methods delineated to enact sentiment analysis over a dataset; Describe the topic modelling task over a dataset; Execute topic modelling using steps with code shown over a dataset;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Participants must have attended the Introduction to Natural Langauge course</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_advNLPpython</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Saliha Minhas</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Describe the boolean retrieval model; Execute the boolean retrieval model over a dataset; Describe the vector space model; Execute the vector space model over a dataset.; Describe how a language model can be used to enact retrieval over a dataset; Execute a language modelling approach to enact retrieval over a dataset; Describe supervised machine learning; Describe pathway of a typical machine learning project; Follow steps in pathway to enact classification over a dataset; Describe sentiment analysis; Describe challenges in a sentiment analysis task; Execute sentiment analysis using methods delineated to enact sentiment analysis over a dataset; Describe the topic modelling task over a dataset; Execute topic modelling using steps with code shown over a dataset</t>
         </is>
       </c>
     </row>
@@ -457,44 +475,52 @@
           <t>Automated Report Production with R</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>6 Hours</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>R is a powerful tool for data analysis and, when coupled with RStudio, the reproducibility feature of coding is further enhanced. Using RStudio and literate programming it is possible to automate the production of reports, replacing tedious and non-reproducible practices of copying and pasting.</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>R users will improve their skills using R markdown to produce automated reports based upon their analyses. Learners will inderstand hw to 'paramaterize' their markdown reports, reducing the need for manual adjustments. Learners will explore the diffreent options for presentation of output to stakeholders.</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> further your knowledge of R markdown: You will further understand the YAML header of a R Markdown document and how to specify parameters that the document will depend on; ;  use functional programming: you will learn how to use the function(al)s map() and walk() from the package purrr to apply a function to the entries of a vector or a list. This will be useful when we read the data in and also to generate all the reports, one per continent, at once; ;  further your coding skills: use conditional if-statements to add information to the report depending on the current parameters. ifelse statements are also used; ;  build on your ggplot2 skills by learning how to produce maps with statistical information in them; ;  get started with writing functions in R: you will be able to write a simple function; ;  learn how to present a table. ;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Intermediate R user.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_ARP</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> further your knowledge of R markdown: You will further understand the YAML header of a R Markdown document and how to specify parameters that the document will depend on; ;  use functional programming: you will learn how to use the function(al)s map() and walk() from the package purrr to apply a function to the entries of a vector or a list. This will be useful when we read the data in and also to generate all the reports, one per continent, at once; ;  further your coding skills: use conditional if-statements to add information to the report depending on the current parameters. ifelse statements are also used; ;  build on your ggplot2 skills by learning how to produce maps with statistical information in them; ;  get started with writing functions in R: you will be able to write a simple function; ;  learn how to present a table. </t>
         </is>
       </c>
     </row>
@@ -504,44 +530,52 @@
           <t>Data Science with R</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12 Hours</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>This course gives the essential knowledge to get started with a data science project in R using the Tidyverse package (https://www.tidyverse.org). We will learn to tell stories with data using the scientific data analysis workflow and analytic tools based on the R system.</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Learners will be able to use the Tidyverse to automate tasks efficiently. They will learn how to use best practice techniques in their workflow from data ingestion through to communication of results.</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Understand the scientific approach to the data analysis workflow and why and how R contributes to the process. ;  Be able to import data into R in different text formats, flat files, excel, SAS, STATA and SPSS files as well as data from the web. ;  Know the concept of tidy data, identify messy features in a data set and tidy it ready for analysis. ;  Use simple exploratory analysis, including visualisation, to understand the data structure and some information it contains and also to detect, be aware of, and possibly correct, data anomalies. ;  Be able to create a basic report  of  data analysis using a R notebook. ;  Work with the Tidyverse packages readr, tidyr, dplyr, stringr, ggplot2, forcats, lubridate, etc. ;                                                           sonjam111               sonjam111                  ;                                                           r-leyshon               r-leyshon                  </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Beginner. Familiar with basic R syntax.</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_DSWR</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Understand the scientific approach to the data analysis workflow and why and how R contributes to the process. ;  Be able to import data into R in different text formats, flat files, excel, SAS, STATA and SPSS files as well as data from the web. ;  Know the concept of tidy data, identify messy features in a data set and tidy it ready for analysis. ;  Use simple exploratory analysis, including visualisation, to understand the data structure and some information it contains and also to detect, be aware of, and possibly correct, data anomalies. ;  Be able to create a basic report  of  data analysis using a R notebook. ;  Work with the Tidyverse packages readr, tidyr, dplyr, stringr, ggplot2, forcats, lubridate, etc. </t>
         </is>
       </c>
     </row>
@@ -551,44 +585,52 @@
           <t>Introduction to ggplot2 and interactive leaflet mapping</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5 Hours</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>This course introduces students to the grammar of graphics and building a plot using ggplot2. In the second part, students are introduced to building interactive maps using leaflet.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Students will become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.; There is a pdf copy of the the ggplot2 and leaflet course slides in the folder slides.; The exercises folder included the accompanying exercises for ggplot2. Leaflet exercises are still being prepared.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>E learning - Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Intermediate</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_ggplot-leaflet-map-training</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Laurie Baker</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Richard Leyshon</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.; There is a pdf copy of the the ggplot2 and leaflet course slides in the folder slides.; The exercises folder included the accompanying exercises for ggplot2. Leaflet exercises are still being prepared.</t>
         </is>
       </c>
     </row>
@@ -598,44 +640,52 @@
           <t>Introduction to R</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10 Hours</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Designed for statistical analysis and reporting, R is a powerful tool for data analysis. This course focuses on the application of key data skills, providing opportunities to build confidence, independence, and resilience. This 1 day course will introduce you to the building blocks of R including objects, vectors, and data frames and will examine common data types (e.g. character, factor). During the course we will also cover data manipulation using dplyr and data visualisation using ggplot with examples from the gapminder dataset.</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>The aim of this course is to equip you with a toolbox to get started with data in R aand Rstudio and to provide a sound foundation from which to continue your learning beyond the classroom.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Familiarise themselves with RStudio and R Notebooks, which is what we’ll use to interact with R. ;  Learn about the simple data structures in R: object, vector, and data frame. ;  Explore R's basic data types = integer, character, numeric, etc. ;  Learn to read data into R. ;  Introduction to data wrangling using the tidyverse set of metapackages. ;  Use the tidyverse verbs to explore the gapminder data set which includes statistics for countries around the world including life expectancy, population, and GDP per capita. ;  Learn to merge datasets using left_join. ;  Create meaningful visualisations of the data using ggplot2. ;  Learn where to go for help. ; Day 1 part 1 &amp; 2; Day 2 part 1 &amp; 2; Day 1: IntroR_exercises.Rmd; Day 2: IntroR_exercises_part2.Rmd; IntroR4IntlDev.html (Self-learning tutorial in html); IntroR4IntlDev.Rmd (R markdown to run exercises); IntroR_part1_slides.pdf (also available in .html); IntroR_part2_slides.pdf (also available in .html); Day 1: IntroR_exercises.Rmd; Day 2: IntroR_exercises_part2.Rmd;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>E learning - Available; Self learning - Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>This courses is aimed at complete beginners with no prior programming experience.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_Intro-R</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Laurie Baker</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Familiarise themselves with RStudio and R Notebooks, which is what we’ll use to interact with R. ;  Learn about the simple data structures in R: object, vector, and data frame. ;  Explore R's basic data types = integer, character, numeric, etc. ;  Learn to read data into R. ;  Introduction to data wrangling using the tidyverse set of metapackages. ;  Use the tidyverse verbs to explore the gapminder data set which includes statistics for countries around the world including life expectancy, population, and GDP per capita. ;  Learn to merge datasets using left_join. ;  Create meaningful visualisations of the data using ggplot2. ;  Learn where to go for help. ; Day 1 part 1 &amp; 2; Day 2 part 1 &amp; 2; Day 1: IntroR_exercises.Rmd; Day 2: IntroR_exercises_part2.Rmd; IntroR4IntlDev.html (Self-learning tutorial in html); IntroR4IntlDev.Rmd (R markdown to run exercises); IntroR_part1_slides.pdf (also available in .html); IntroR_part2_slides.pdf (also available in .html); Day 1: IntroR_exercises.Rmd; Day 2: IntroR_exercises_part2.Rmd</t>
         </is>
       </c>
     </row>
@@ -645,44 +695,52 @@
           <t>Introduction to Natural Language Programming with Python</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>6 Hours</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Participants should gain competancy in using core techniques to handle natural language content to undertake analysis to detect patterns and derive insights for development of applications like mentioned in course summary</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.; Produce clusters using the k-means algorithm to uncover patterns in a corpus; Transform text to vectors using approaches delineated.; Produce word embeddings on a corpus; Calculate the probability of a sentence using a language modelling approach;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Competency in using the Python Programming language to perform basic data manipulation is reqiured.</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_introNLPpython</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Saliha Minhas</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Kaveh Jahanshahi</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.; Produce clusters using the k-means algorithm to uncover patterns in a corpus; Transform text to vectors using approaches delineated.; Produce word embeddings on a corpus; Calculate the probability of a sentence using a language modelling approach</t>
         </is>
       </c>
     </row>
@@ -692,44 +750,52 @@
           <t>Introduction to Python Programming</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8">
+        <v>1.1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10 Hours</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>This course is delivered through the Jupyter notebook application. It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists, dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types to compose code with selection and iteration constructs.  To promote modular and readable code the set-up and use of functions with parameters are also covered. Specialised knowledge in data analysis is then developed through a comprehensive overview of the Pandas library. The two main data structures in this library – the series and dataframe and associated methods are explained with clarifying examples on how to select, filter, aggregate and merge data. Keys tasks like handling null values, applying functions, plotting are also highlighted.  Each section has exercises for participants to attempt to consolidate their learning.</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Participants should attain a good understanding of basic data types in Python and associated methods and constructs that can be applied to them. They should also become knowledgeable in how to deal with tabular data through using the specialised data structures found in the Pandas library and how to perform key analysis through methods available in this library.</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code; Describe specialised data structures - the series and dataframe in the Pandas library; Select, filter, aggregate, merge data in the Pandas dataframe; Execute specific operations to handle null values and apply functions.; Plot data in a dataframe column(s).;                                         ;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>E learning - Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>No previous experience in coding is required though a  basic digital literacy assumed.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_intropython</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Saliha Minhas</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Richard Leyshon, Kaveh Jahanshahi</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code; Describe specialised data structures - the series and dataframe in the Pandas library; Select, filter, aggregate, merge data in the Pandas dataframe; Execute specific operations to handle null values and apply functions.; Plot data in a dataframe column(s).</t>
         </is>
       </c>
     </row>
@@ -739,44 +805,49 @@
           <t>Theory in Machine Learning</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>course duration not found</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>course summary not found</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>learning objective not found</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>description of what the project is; instruction on how to install the tool (if applicable); detailed instructions on basic use; a demo of the code; Low; Medium; High; Critical; Legal!; Data!; Engagement!; Resource!; Tech!; CODE_OF_CONDUCT.md: a statement from the Contributor Covenant regarding what is and isn't acceptable behaviour for contributors; CONTRIBUTING.md: guidelines for how contributions should be made to the work, this should be updated when the work is made public; README.md: this document, every repository should have one and it acts as the main landing page for your repository; LICENSE: the UK public sector usually operate under two different licensing schemes. The most common for code is the MIT license which is included in this repo. Alternatively there is an Open Government license and a description of what OpenGov enforces can be found here.; .github: this directory allows the user to specify templates for contribution types, included in this repository are a bug fix submission template, a feature request template and a pull request template. Each of them includes a series of tickboxes which you can use to help you decide whether or not the submission is suitable.; .gitignore: this file allows you to specify which directories, files and globbed file types are to be ignored as part of the diffs being managed by git. This allows you to have your data in the same directory structure as your code without it needing to be pushed and pulled along with it. If you have data which you do need to manage I would highly advise the use of git-annex ahead of including data files in your repository (unless they are small).</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>No course type detected</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Skill level not found</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_ML_theory</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>lead developer not found</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Course reviewer not found</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>README.md: this document, every repository should have one and it acts as the main landing page for your repository; LICENSE: the UK public sector usually operate under two different licensing schemes. The most common for code is the MIT license which is included in this repo. Alternatively there is an Open Government license and a description of what OpenGov enforces can be found here.; .github: this directory allows the user to specify templates for contribution types, included in this repository are a bug fix submission template, a feature request template and a pull request template. Each of them includes a series of tickboxes which you can use to help you decide whether or not the submission is suitable.; .gitignore: this file allows you to specify which directories, files and globbed file types are to be ignored as part of the diffs being managed by git. This allows you to have your data in the same directory structure as your code without it needing to be pushed and pulled along with it. If you have data which you do need to manage I would highly advise the use of git-annex ahead of including data files in your repository (unless they are small).</t>
         </is>
       </c>
     </row>
@@ -786,44 +857,52 @@
           <t>Natural Language Processing with R</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>8 Hours</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language (texts). Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.;                                         ;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Kaveh Jahanshahi</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
         </is>
       </c>
     </row>
@@ -833,44 +912,52 @@
           <t>Statistics for Data Science</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>18 Hours</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>This course introduces the basics of carrying out a statistical analysis in Python. It covers exploratory data analysis, constructing and interpreting linear and generalized linear models, and introduces Bayesian modelling.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in A continuous variable A categorical variable  How to use plots to explore covariation between Two categorical variables Two continuous variables A categorical and continuous variable.  ; How to use plots to explore variation in A continuous variable A categorical variable ; A continuous variable; A categorical variable; How to use plots to explore covariation between Two categorical variables Two continuous variables A categorical and continuous variable. ; Two categorical variables; Two continuous variables; A categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.; Exploratory Data Analysis (Chapter 1); Generalized Linear Models (Chapter 3); Intro_Bayes (Chapter 4);                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Laurie Baker, Dan Lewis</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in A continuous variable A categorical variable  How to use plots to explore covariation between Two categorical variables Two continuous variables A categorical and continuous variable.  ; How to use plots to explore variation in A continuous variable A categorical variable ; A continuous variable; A categorical variable; How to use plots to explore covariation between Two categorical variables Two continuous variables A categorical and continuous variable. ; Two categorical variables; Two continuous variables; A categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.; Exploratory Data Analysis (Chapter 1); Generalized Linear Models (Chapter 3); Intro_Bayes (Chapter 4)</t>
         </is>
       </c>
     </row>
@@ -880,44 +967,52 @@
           <t>Version Control with Git: Github</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4 Hours</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>Publications that make the used code available have generally higher impact than publications where code is not available. One important tool for code quality and code sharing is a version control system (VCS). A version control system is a tool that manages changes made to the files and directories in a project. Git, together with GitHub, is one such VCS tool.</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document;                                         ;                                         </t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Intermediate / Advanced</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
         </is>
       </c>
     </row>
@@ -927,44 +1022,52 @@
           <t>Version controlled RStudio projects</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4 Hours</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>RStudio has the ability to use version control for R projects using a very easy to use graphical interface. In this course we will introduce how R Studio has integrated Git version control into its interface. This allows developers to efficiently track changes in their code over time and effectively collaborate with a team of programmers. This course explains how to use the Git workflow to revise and track changes to an r markdown document, ultimately publishing your own version to web.</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Learners will be able to use R Studio's integrated Git features to improve their ability to track changes and collaborate in their code.</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE;                                                           sonjam111               sonjam111                  ;                                                           r-leyshon               r-leyshon                  </t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Intermediate R user.</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_Version-controlled-RStudio-projects</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Pending</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
error handling as requested by GP
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -440,7 +440,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Describe the boolean retrieval model; Execute the boolean retrieval model over a dataset; Describe the vector space model; Execute the vector space model over a dataset.; Describe how a language model can be used to enact retrieval over a dataset; Execute a language modelling approach to enact retrieval over a dataset; Describe supervised machine learning; Describe pathway of a typical machine learning project; Follow steps in pathway to enact classification over a dataset; Describe sentiment analysis; Describe challenges in a sentiment analysis task; Execute sentiment analysis using methods delineated to enact sentiment analysis over a dataset; Describe the topic modelling task over a dataset; Execute topic modelling using steps with code shown over a dataset;                                                           salihadfid1               salihadfid1                  ;                                                           r-leyshon               r-leyshon                  </t>
+          <t>Describe the boolean retrieval model; Execute the boolean retrieval model over a dataset; Describe the vector space model; Execute the vector space model over a dataset.; Describe how a language model can be used to enact retrieval over a dataset; Execute a language modelling approach to enact retrieval over a dataset; Describe supervised machine learning; Describe pathway of a typical machine learning project; Follow steps in pathway to enact classification over a dataset; Describe sentiment analysis; Describe challenges in a sentiment analysis task; Execute sentiment analysis using methods delineated to enact sentiment analysis over a dataset; Describe the topic modelling task over a dataset; Execute topic modelling using steps with code shown over a dataset</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> further your knowledge of R markdown: You will further understand the YAML header of a R Markdown document and how to specify parameters that the document will depend on; ;  use functional programming: you will learn how to use the function(al)s map() and walk() from the package purrr to apply a function to the entries of a vector or a list. This will be useful when we read the data in and also to generate all the reports, one per continent, at once; ;  further your coding skills: use conditional if-statements to add information to the report depending on the current parameters. ifelse statements are also used; ;  build on your ggplot2 skills by learning how to produce maps with statistical information in them; ;  get started with writing functions in R: you will be able to write a simple function; ;  learn how to present a table. ;                                                           sonjam111               sonjam111                  ;                                                           r-leyshon               r-leyshon                  </t>
+          <t xml:space="preserve"> further your knowledge of R markdown: You will further understand the YAML header of a R Markdown document and how to specify parameters that the document will depend on; ;  use functional programming: you will learn how to use the function(al)s map() and walk() from the package purrr to apply a function to the entries of a vector or a list. This will be useful when we read the data in and also to generate all the reports, one per continent, at once; ;  further your coding skills: use conditional if-statements to add information to the report depending on the current parameters. ifelse statements are also used; ;  build on your ggplot2 skills by learning how to produce maps with statistical information in them; ;  get started with writing functions in R: you will be able to write a simple function; ;  learn how to present a table. </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Understand the scientific approach to the data analysis workflow and why and how R contributes to the process. ;  Be able to import data into R in different text formats, flat files, excel, SAS, STATA and SPSS files as well as data from the web. ;  Know the concept of tidy data, identify messy features in a data set and tidy it ready for analysis. ;  Use simple exploratory analysis, including visualisation, to understand the data structure and some information it contains and also to detect, be aware of, and possibly correct, data anomalies. ;  Be able to create a basic report  of  data analysis using a R notebook. ;  Work with the Tidyverse packages readr, tidyr, dplyr, stringr, ggplot2, forcats, lubridate, etc. ;                                         ;                                         </t>
+          <t xml:space="preserve"> Understand the scientific approach to the data analysis workflow and why and how R contributes to the process. ;  Be able to import data into R in different text formats, flat files, excel, SAS, STATA and SPSS files as well as data from the web. ;  Know the concept of tidy data, identify messy features in a data set and tidy it ready for analysis. ;  Use simple exploratory analysis, including visualisation, to understand the data structure and some information it contains and also to detect, be aware of, and possibly correct, data anomalies. ;  Be able to create a basic report  of  data analysis using a R notebook. ;  Work with the Tidyverse packages readr, tidyr, dplyr, stringr, ggplot2, forcats, lubridate, etc. </t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.; There is a pdf copy of the the ggplot2 and leaflet course slides in the folder slides.; The exercises folder included the accompanying exercises for ggplot2. Leaflet exercises are still being prepared.</t>
+          <t>become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -660,7 +660,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Familiarise themselves with RStudio and R Notebooks, which is what we’ll use to interact with R. ;  Learn about the simple data structures in R: object, vector, and data frame. ;  Explore R's basic data types = integer, character, numeric, etc. ;  Learn to read data into R. ;  Introduction to data wrangling using the tidyverse set of metapackages. ;  Use the tidyverse verbs to explore the gapminder data set which includes statistics for countries around the world including life expectancy, population, and GDP per capita. ;  Learn to merge datasets using left_join. ;  Create meaningful visualisations of the data using ggplot2. ;  Learn where to go for help. ; Day 1 part 1 &amp; 2; Day 2 part 1 &amp; 2; Day 1: IntroR_exercises.Rmd; Day 2: IntroR_exercises_part2.Rmd; IntroR4IntlDev.html (Self-learning tutorial in html); IntroR4IntlDev.Rmd (R markdown to run exercises); IntroR_part1_slides.pdf (also available in .html); IntroR_part2_slides.pdf (also available in .html); Day 1: IntroR_exercises.Rmd; Day 2: IntroR_exercises_part2.Rmd;                                         ;                                         </t>
+          <t xml:space="preserve"> Familiarise themselves with RStudio and R Notebooks, which is what we’ll use to interact with R. ;  Learn about the simple data structures in R: object, vector, and data frame. ;  Explore R's basic data types = integer, character, numeric, etc. ;  Learn to read data into R. ;  Introduction to data wrangling using the tidyverse set of metapackages. ;  Use the tidyverse verbs to explore the gapminder data set which includes statistics for countries around the world including life expectancy, population, and GDP per capita. ;  Learn to merge datasets using left_join. ;  Create meaningful visualisations of the data using ggplot2. ;  Learn where to go for help. </t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.; Produce clusters using the k-means algorithm to uncover patterns in a corpus; Transform text to vectors using approaches delineated.; Produce word embeddings on a corpus; Calculate the probability of a sentence using a language modelling approach;                                         ;                                         </t>
+          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.; Produce clusters using the k-means algorithm to uncover patterns in a corpus; Transform text to vectors using approaches delineated.; Produce word embeddings on a corpus; Calculate the probability of a sentence using a language modelling approach</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code; Describe specialised data structures - the series and dataframe in the Pandas library; Select, filter, aggregate, merge data in the Pandas dataframe; Execute specific operations to handle null values and apply functions.; Plot data in a dataframe column(s).;                                         ;                                         ;                                         </t>
+          <t>Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code; Describe specialised data structures - the series and dataframe in the Pandas library; Select, filter, aggregate, merge data in the Pandas dataframe; Execute specific operations to handle null values and apply functions.; Plot data in a dataframe column(s).</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>description of what the project is; instruction on how to install the tool (if applicable); detailed instructions on basic use; a demo of the code; Low; Medium; High; Critical; Legal!; Data!; Engagement!; Resource!; Tech!; CODE_OF_CONDUCT.md: a statement from the Contributor Covenant regarding what is and isn't acceptable behaviour for contributors; CONTRIBUTING.md: guidelines for how contributions should be made to the work, this should be updated when the work is made public; README.md: this document, every repository should have one and it acts as the main landing page for your repository; LICENSE: the UK public sector usually operate under two different licensing schemes. The most common for code is the MIT license which is included in this repo. Alternatively there is an Open Government license and a description of what OpenGov enforces can be found here.; .github: this directory allows the user to specify templates for contribution types, included in this repository are a bug fix submission template, a feature request template and a pull request template. Each of them includes a series of tickboxes which you can use to help you decide whether or not the submission is suitable.; .gitignore: this file allows you to specify which directories, files and globbed file types are to be ignored as part of the diffs being managed by git. This allows you to have your data in the same directory structure as your code without it needing to be pushed and pulled along with it. If you have data which you do need to manage I would highly advise the use of git-annex ahead of including data files in your repository (unless they are small).</t>
+          <t>Learning Objectives Not Found</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.;                                         ;                                         ;                                         </t>
+          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in A continuous variable A categorical variable  How to use plots to explore covariation between Two categorical variables Two continuous variables A categorical and continuous variable.  ; How to use plots to explore variation in A continuous variable A categorical variable ; A continuous variable; A categorical variable; How to use plots to explore covariation between Two categorical variables Two continuous variables A categorical and continuous variable. ; Two categorical variables; Two continuous variables; A categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.; Exploratory Data Analysis (Chapter 1); Generalized Linear Models (Chapter 3); Intro_Bayes (Chapter 4);                                         ;                                         </t>
+          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document;                                                           sonjam111               sonjam111                  ;                                                           r-leyshon               r-leyshon                  </t>
+          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE;                                         ;                                         </t>
+          <t>Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">

</xml_diff>

<commit_message>
removal of old zip folders on script execution
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -425,12 +425,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>This course will focus on four key topics in Natural Language Processing: information retrieval, classification, sentiment analysis and topic modelling. Information retrieval covers the building blocks of a search engine - the inverted index and maps out in detail with both illustrations and code how an information retrieval application can be built. Three disparate, classical approaches will be examined to fulfil this objective. Classification will then be outlined, focusing on its supervised machine learning foundations. A real-world classification problem of news classification will be illustrated using a BBC news dataset. Classification will again be enacted to undertake sentiment analysis. Key challanges in the field of sentiment analysis will also be explored.  Topic Modelling as the name suggests is a process to automatically identify topics present in a datset. The course will demostrate from a practical perspective how this can be attained.</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -480,12 +480,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R is a powerful tool for data analysis and, when coupled with RStudio, the reproducibility feature of coding is further enhanced. Using RStudio and literate programming it is possible to automate the production of reports, replacing tedious and non-reproducible practices of copying and pasting.</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,12 +535,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>This course gives the essential knowledge to get started with a data science project in R using the Tidyverse package (https://www.tidyverse.org). We will learn to tell stories with data using the scientific data analysis workflow and analytic tools based on the R system.</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -590,12 +590,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>This course introduces students to the grammar of graphics and building a plot using ggplot2. In the second part, students are introduced to building interactive maps using leaflet.</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -645,12 +645,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Designed for statistical analysis and reporting, R is a powerful tool for data analysis. This course focuses on the application of key data skills, providing opportunities to build confidence, independence, and resilience. This 1 day course will introduce you to the building blocks of R including objects, vectors, and data frames and will examine common data types (e.g. character, factor). During the course we will also cover data manipulation using dplyr and data visualisation using ggplot with examples from the gapminder dataset.</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -700,12 +700,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6 Hours</t>
+          <t>Course Objective</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
+          <t>Lead Developer Participants should gain competancy in using core techniques to handle natural language content to undertake analysis to detect patterns and derive insights for development of applications like mentioned in course summary Course Objective Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -755,12 +755,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>This course is delivered through the Jupyter notebook application. It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists, dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types to compose code with selection and iteration constructs.  To promote modular and readable code the set-up and use of functions with parameters are also covered. Specialised knowledge in data analysis is then developed through a comprehensive overview of the Pandas library. The two main data structures in this library – the series and dataframe and associated methods are explained with clarifying examples on how to select, filter, aggregate and merge data. Keys tasks like handling null values, applying functions, plotting are also highlighted.  Each section has exercises for participants to attempt to consolidate their learning.</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -862,12 +862,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>8 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language (texts). Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -917,12 +917,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>18 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>This course introduces the basics of carrying out a statistical analysis in Python. It covers exploratory data analysis, constructing and interpreting linear and generalized linear models, and introduces Bayesian modelling.</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -972,12 +972,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Publications that make the used code available have generally higher impact than publications where code is not available. One important tool for code quality and code sharing is a version control system (VCS). A version control system is a tool that manages changes made to the files and directories in a project. Git, together with GitHub, is one such VCS tool.</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1027,12 +1027,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4 Hours</t>
+          <t>course duration not found</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>RStudio has the ability to use version control for R projects using a very easy to use graphical interface. In this course we will introduce how R Studio has integrated Git version control into its interface. This allows developers to efficiently track changes in their code over time and effectively collaborate with a team of programmers. This course explains how to use the Git workflow to revise and track changes to an r markdown document, ultimately publishing your own version to web.</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">

</xml_diff>

<commit_message>
version 1.5, exception handling for repos with non-standard readmes.
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -490,7 +490,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R users will improve their skills using R markdown to produce automated reports based upon their analyses. Learners will inderstand hw to 'paramaterize' their markdown reports, reducing the need for manual adjustments. Learners will explore the diffreent options for presentation of output to stakeholders.</t>
+          <t>R users will improve their skills using R markdown to produce automated reports based upon their analyses. Learners will understand how to 'paramaterize' their markdown reports, reducing the need for manual adjustments. Learners will explore the diffreent options for presentation of output to stakeholders.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -665,7 +665,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning - Available; Face to face - Available</t>
+          <t>E learning - Available; Self learning - Available Soon; Face to face - Available</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -760,22 +760,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Participants should attain a good understanding of basic data types in Python and associated methods and constructs that can be applied to them. They should also become knowledgeable in how to deal with tabular data through using the specialised data structures found in the Pandas library and how to perform key analysis through methods available in this library.</t>
+          <t>Participants should attain a good understanding of basic data types in Python and associated methods and constructs that can be applied to them.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code; Describe specialised data structures - the series and dataframe in the Pandas library; Select, filter, aggregate, merge data in the Pandas dataframe; Execute specific operations to handle null values and apply functions.; Plot data in a dataframe column(s).</t>
+          <t>Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning - Not Available; Face to face - Available</t>
+          <t>E learning - Available; Self learning - Available Soon; Face to face - Available</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -802,8 +802,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Theory in Machine Learning</t>
-        </is>
+          <t>Natural Language Processing with R</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -812,49 +815,49 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>learning objective not found</t>
+          <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Learning Objectives Not Found</t>
+          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>No course type detected</t>
+          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Skill level not found</t>
+          <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_ML_theory</t>
+          <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>lead developer not found</t>
+          <t>Sonia Mazzi</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Course reviewer not found</t>
+          <t>Kaveh Jahanshahi</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Natural Language Processing with R</t>
+          <t>Statistics for Data Science</t>
         </is>
       </c>
       <c r="B10">
@@ -872,44 +875,44 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
+          <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
+          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
+          <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
+          <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
+          <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Sonia Mazzi</t>
+          <t>Laurie Baker, Dan Lewis</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Kaveh Jahanshahi</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Statistics for Data Science</t>
+          <t>Version Control with Git: Github</t>
         </is>
       </c>
       <c r="B11">
@@ -922,37 +925,37 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>course summary not found</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
+          <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
+          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
+          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
+          <t>Intermediate / Advanced</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
+          <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Laurie Baker, Dan Lewis</t>
+          <t>Sonia Mazzi</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -964,7 +967,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Version Control with Git: Github</t>
+          <t>Version controlled RStudio projects</t>
         </is>
       </c>
       <c r="B12">
@@ -982,12 +985,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
+          <t>Learners will be able to use R Studio's integrated Git features to improve their ability to track changes and collaborate in their code.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
+          <t>Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -997,12 +1000,12 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Intermediate / Advanced</t>
+          <t>Intermediate R user.</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
+          <t>https://github.com/datasciencecampus/DSCA_Version-controlled-RStudio-projects</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1011,61 +1014,6 @@
         </is>
       </c>
       <c r="K12" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Version controlled RStudio projects</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>course duration not found</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>course summary not found</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Learners will be able to use R Studio's integrated Git features to improve their ability to track changes and collaborate in their code.</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Intermediate R user.</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>https://github.com/datasciencecampus/DSCA_Version-controlled-RStudio-projects</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Sonia Mazzi</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>

</xml_diff>

<commit_message>
error handling with course duration paragpraph nodes  - website structure change
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -425,12 +425,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>6 Hours</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>This course will focus on four key topics in Natural Language Processing: information retrieval, classification, sentiment analysis and topic modelling. Information retrieval covers the building blocks of a search engine - the inverted index and maps out in detail with both illustrations and code how an information retrieval application can be built. Three disparate, classical approaches will be examined to fulfil this objective. Classification will then be outlined, focusing on its supervised machine learning foundations. A real-world classification problem of news classification will be illustrated using a BBC news dataset. Classification will again be enacted to undertake sentiment analysis. Key challanges in the field of sentiment analysis will also be explored.  Topic Modelling as the name suggests is a process to automatically identify topics present in a datset. The course will demostrate from a practical perspective how this can be attained.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -480,12 +480,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>6 Hours</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>R is a powerful tool for data analysis and, when coupled with RStudio, the reproducibility feature of coding is further enhanced. Using RStudio and literate programming it is possible to automate the production of reports, replacing tedious and non-reproducible practices of copying and pasting.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,12 +535,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>12 Hours</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>This course gives the essential knowledge to get started with a data science project in R using the Tidyverse package (https://www.tidyverse.org). We will learn to tell stories with data using the scientific data analysis workflow and analytic tools based on the R system.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -590,12 +590,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>5 Hours</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>This course introduces students to the grammar of graphics and building a plot using ggplot2. In the second part, students are introduced to building interactive maps using leaflet.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -645,12 +645,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>10 Hours</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>Designed for statistical analysis and reporting, R is a powerful tool for data analysis. This course focuses on the application of key data skills, providing opportunities to build confidence, independence, and resilience. This 1 day course will introduce you to the building blocks of R including objects, vectors, and data frames and will examine common data types (e.g. character, factor). During the course we will also cover data manipulation using dplyr and data visualisation using ggplot with examples from the gapminder dataset.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -700,12 +700,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Course Objective</t>
+          <t>6 Hours</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Lead Developer Participants should gain competancy in using core techniques to handle natural language content to undertake analysis to detect patterns and derive insights for development of applications like mentioned in course summary Course Objective Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
+          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -755,12 +755,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>6 to 8 Hours</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>This course is delivered through the Jupyter notebook application. It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists, dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types to compose code with selection and iteration constructs.  To promote modular and readable code the set-up and use of functions with parameters are also covered.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -802,7 +802,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Natural Language Processing with R</t>
+          <t>Fundemental theories in Machine Learning</t>
         </is>
       </c>
       <c r="B9">
@@ -810,22 +810,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>8 Hours</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>This course covers the fundemental topics in machine learning and prepare audience for more advanced topics (e.g. image processing, NLP, and deep learning) and practical courses such as training and application of machine learning algorithms in R and Python. The course includes combination of graphical presentation and intuition and essential mathematical notations.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
+          <t>This course aims to:</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
+          <t>Provide a thorough introduction into probabilityb theory and statistical inference including maximum-likelihood and Bayesian approaches; Introduce supervised learning methods: linear and nonlinear regressions and classification algorithms; Introduce unsupervised learning methods: clustering, and dimensionality reduction; Breif introduction to Directed Graphical Models with a case study/example.; be able to describe the diffence between frequentist and bayessian statistics; Undrestand the fundementals of probability theory, bayesian rule and inference, and the characteristics of major probability distributions.; Get a good undrestanding of major supervised learning algorithms specifically linear in parameter regression, bayesian linear regression, and classification methods.; Get a good understanding of main unsupervised learning algorithms specifically clustering and data dimensionality reduction algorithms.; Get familiar with directed graphical method as a technique of combining supervised and unsupervised learning into one modelling framework; be prepared to built on their current knowledge or take on more advanced courses such as application of machine learning techniques in natural language processing; be prepared to apply their knowledge through formulating machine learning problems and coding using standard libraries (e.g. in R and Python)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -835,29 +835,29 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
+          <t>Some basic knowledge in linear algebra and statistics is expected.</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
+          <t>https://github.com/datasciencecampus/DSCA_ML_theory</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Sonia Mazzi</t>
+          <t>Kaveh Jahanshahi</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Kaveh Jahanshahi</t>
+          <t>Laurie Baker  Isabela Breton</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Statistics for Data Science</t>
+          <t>Natural Language Processing with R</t>
         </is>
       </c>
       <c r="B10">
@@ -865,54 +865,54 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>8 Hours</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language (texts). Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
+          <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
+          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
+          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
+          <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
+          <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Laurie Baker, Dan Lewis</t>
+          <t>Sonia Mazzi</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Kaveh Jahanshahi</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Version Control with Git: Github</t>
+          <t>Introduction to Reproducibility</t>
         </is>
       </c>
       <c r="B11">
@@ -920,22 +920,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>Course Summary</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>Introduction to reproducibility including, what is a reproducible analytical pipeline, writing "good code" and creating a reproducible report.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
+          <t>Lead Developer Course Objective</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -945,17 +945,17 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Intermediate / Advanced</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
+          <t>https://github.com/datasciencecampus/DSCA_reproducibility</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Sonia Mazzi</t>
+          <t>Laurie L. Baker Richard Leyshon</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -967,7 +967,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Version controlled RStudio projects</t>
+          <t>Statistics for Data Science</t>
         </is>
       </c>
       <c r="B12">
@@ -975,45 +975,155 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>course duration not found</t>
+          <t>18 Hours</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>course summary not found</t>
+          <t>This course introduces the basics of carrying out a statistical analysis in Python. It covers exploratory data analysis, constructing and interpreting linear and generalized linear models, and introduces Bayesian modelling.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Laurie Baker, Dan Lewis</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Version Control with Git: Github</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4 Hours</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Publications that make the used code available have generally higher impact than publications where code is not available. One important tool for code quality and code sharing is a version control system (VCS). A version control system is a tool that manages changes made to the files and directories in a project. Git, together with GitHub, is one such VCS tool.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Intermediate / Advanced</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Sonia Mazzi</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Version controlled RStudio projects</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4 Hours</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>RStudio has the ability to use version control for R projects using a very easy to use graphical interface. In this course we will introduce how R Studio has integrated Git version control into its interface. This allows developers to efficiently track changes in their code over time and effectively collaborate with a team of programmers. This course explains how to use the Git workflow to revise and track changes to an r markdown document, ultimately publishing your own version to web.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Learners will be able to use R Studio's integrated Git features to improve their ability to track changes and collaborate in their code.</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Intermediate R user.</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_Version-controlled-RStudio-projects</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>

</xml_diff>

<commit_message>
version 2.6 initial commit. Licence metadata reintroduced from repo metadata (github api)
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,6 +413,11 @@
           <t>course_reviewer</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>license_name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -468,6 +473,11 @@
           <t>Pending</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -523,6 +533,11 @@
           <t>Pending</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -578,6 +593,11 @@
           <t>Pending</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -633,6 +653,11 @@
           <t>Richard Leyshon</t>
         </is>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -688,6 +713,11 @@
           <t>Pending</t>
         </is>
       </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -743,6 +773,11 @@
           <t>Kaveh Jahanshahi</t>
         </is>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -798,6 +833,11 @@
           <t>Richard Leyshon, Kaveh Jahanshahi</t>
         </is>
       </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -820,12 +860,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>This course aims to:</t>
+          <t>Provide a thorough introduction into probability theory and statistical inference including maximum-likelihood and Bayesian approaches. Introduce supervised learning methods: linear and nonlinear regressions and classification algorithms. Introduce unsupervised learning methods: clustering, and dimensionality reduction. Brief introduction to Directed Graphical Models with a case study/example.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Provide a thorough introduction into probabilityb theory and statistical inference including maximum-likelihood and Bayesian approaches; Introduce supervised learning methods: linear and nonlinear regressions and classification algorithms; Introduce unsupervised learning methods: clustering, and dimensionality reduction; Breif introduction to Directed Graphical Models with a case study/example.; be able to describe the diffence between frequentist and bayessian statistics; Undrestand the fundementals of probability theory, bayesian rule and inference, and the characteristics of major probability distributions.; Get a good undrestanding of major supervised learning algorithms specifically linear in parameter regression, bayesian linear regression, and classification methods.; Get a good understanding of main unsupervised learning algorithms specifically clustering and data dimensionality reduction algorithms.; Get familiar with directed graphical method as a technique of combining supervised and unsupervised learning into one modelling framework; be prepared to built on their current knowledge or take on more advanced courses such as application of machine learning techniques in natural language processing; be prepared to apply their knowledge through formulating machine learning problems and coding using standard libraries (e.g. in R and Python)</t>
+          <t>Be able to describe the diffence between frequentist and bayesian statistics; Understand the fundementals of probability theory, bayesian rule and inference, and the characteristics of major probability distributions.; Get a good understanding of major supervised learning algorithms specifically linear in parameter regression, bayesian linear regression, and classification methods.; Get a good understanding of main unsupervised learning algorithms specifically clustering and data dimensionality reduction algorithms.; Get familiar with directed graphical method as a technique of combining supervised and unsupervised learning into one modelling framework; be prepared to build on their current knowledge or take on more advanced courses such as application of machine learning techniques in natural language processing; be prepared to apply their knowledge through formulating machine learning problems and coding using standard libraries (e.g. in R and Python)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -851,6 +891,11 @@
       <c r="K9" t="inlineStr">
         <is>
           <t>Laurie Baker  Isabela Breton</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>MIT License</t>
         </is>
       </c>
     </row>
@@ -908,6 +953,11 @@
           <t>Kaveh Jahanshahi</t>
         </is>
       </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -920,22 +970,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Course Summary</t>
+          <t>6 Hours</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Introduction to reproducibility including, what is a reproducible analytical pipeline, writing "good code" and creating a reproducible report.</t>
+          <t>Introduction to reproducibility. What is a reproducible analytical pipeline (RAP), writing "good code" and creating a reproducible report.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Lead Developer Course Objective</t>
+          <t>Participants should gain an awareness of the importance of reproducibility in their work. Learners will also gain experience of linting code in Python and using parameterised reports in R markdown.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>represent pipelines and identify opportunities to automate; consider adherance to a programming style guide; use linting software to standardise Python scripts; use parameterised R markdown reports to improve the efficiency of report production.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -945,7 +995,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Basic familiarity with Python and R programming is assumed.</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -961,6 +1011,11 @@
       <c r="K11" t="inlineStr">
         <is>
           <t>Pending</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>NULL</t>
         </is>
       </c>
     </row>
@@ -1018,6 +1073,11 @@
           <t>Pending</t>
         </is>
       </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1073,6 +1133,11 @@
           <t>Pending</t>
         </is>
       </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1126,6 +1191,11 @@
       <c r="K14" t="inlineStr">
         <is>
           <t>Pending</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>NULL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
stler & linter on scripts
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -735,7 +735,15 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
+          <t>Natural Language Processing is a sub-field of Artificial Intelligence.
+It is used for processing and analysing large amounts of natural language.
+Some applications include search engines (Google), text classification (spam filters),
+identifying sentiments for a product (sentiment analysis), methods for discovering
+abstract topics in a collection of documents (topic modelling) and machine translation technologies.
+Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics,
+and application of feature engineering techniques to transform textual data into a numerical representation.
+Key techniques such as word embeddings and language modelling are also introduced as well as illustrations
+as to how they can be performed over a dataset.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -795,12 +803,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>This course is delivered through the Jupyter notebook application. It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists, dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types to compose code with selection and iteration constructs.  To promote modular and readable code the set-up and use of functions with parameters are also covered.</t>
+          <t>This course is delivered through the Jupyter notebook application.
+It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists,
+dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types
+to compose code with selection and iteration constructs.  To promote modular and readable code the set-up
+and use of functions with parameters are also covered.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Participants should attain a good understanding of basic data types in Python and associated methods and constructs that can be applied to them.</t>
+          <t>Participants should attain a good understanding of basic data types in Python and associated methods
+and constructs that can be applied to them.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -830,7 +843,8 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Richard Leyshon, Kaveh Jahanshahi</t>
+          <t>Richard Leyshon,
+Kaveh Jahanshahi</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -890,7 +904,8 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Laurie Baker  Isabela Breton</t>
+          <t>Laurie Baker 
+Isabela Breton</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -915,7 +930,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language (texts). Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
+          <t>Natural Language Processing is a sub-field of Artificial Intelligence.
+It is used for processing and analysing large amounts of natural language (texts).
+Some applications include search engines (Google), text classification (spam filters),
+identifying sentiments for a product (sentiment analysis), methods for discovering
+abstract topics in a collection of documents (topic modelling) and machine translation technologies.
+In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1005,7 +1025,8 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Laurie L. Baker Richard Leyshon</t>
+          <t>Laurie L. Baker
+Richard Leyshon</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">

</xml_diff>

<commit_message>
v1.6 - agreed pattern in repo description results in filtering out from dataframe
</commit_message>
<xml_diff>
--- a/output_data/course_catalogue.xlsx
+++ b/output_data/course_catalogue.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,7 +542,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Data Science with R</t>
+          <t>Data Visualisation in R</t>
         </is>
       </c>
       <c r="B4">
@@ -550,59 +550,59 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12 Hours</t>
+          <t>3 Hours</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>This course gives the essential knowledge to get started with a data science project in R using the Tidyverse package (https://www.tidyverse.org). We will learn to tell stories with data using the scientific data analysis workflow and analytic tools based on the R system.</t>
+          <t>This course introduces students to the grammar of graphics and building a plot using ggplot2.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Learners will be able to use the Tidyverse to automate tasks efficiently. They will learn how to use best practice techniques in their workflow from data ingestion through to communication of results.</t>
+          <t>Students will become familiar with how a plot is built using ggplot learn to customise and create different plots.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Understand the scientific approach to the data analysis workflow and why and how R contributes to the process. ;  Be able to import data into R in different text formats, flat files, excel, SAS, STATA and SPSS files as well as data from the web. ;  Know the concept of tidy data, identify messy features in a data set and tidy it ready for analysis. ;  Use simple exploratory analysis, including visualisation, to understand the data structure and some information it contains and also to detect, be aware of, and possibly correct, data anomalies. ;  Be able to create a basic report  of  data analysis using a R notebook. ;  Work with the Tidyverse packages readr, tidyr, dplyr, stringr, ggplot2, forcats, lubridate, etc. </t>
+          <t>Be familiar with how a construct a basic plot using layers in ggplot.; Understand how variables in the data are used to determine aesthetics of the plot.; Be familiar with the concepts of tidy data.; Understand the connection between different geoms and the type of plot they produce (e.g. geom_line, geom_point).; Understand how to customise a plot using labs, theme, facet.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
+          <t>Online learning - Not Available; Independent learning - Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Beginner. Familiar with basic R syntax.</t>
+          <t>Intermediate</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_DSWR</t>
+          <t>https://github.com/datasciencecampus/DSCA_data_visualisation_in_r</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Sonia Mazzi</t>
+          <t>Laurie Baker</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Richard Leyshon</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Introduction to ggplot2 and interactive leaflet mapping</t>
+          <t>Data Science with R</t>
         </is>
       </c>
       <c r="B5">
@@ -610,107 +610,107 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5 Hours</t>
+          <t>12 Hours</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>This course introduces students to the grammar of graphics and building a plot using ggplot2. In the second part, students are introduced to building interactive maps using leaflet.</t>
+          <t>This course gives the essential knowledge to get started with a data science project in R using the Tidyverse package (https://www.tidyverse.org). We will learn to tell stories with data using the scientific data analysis workflow and analytic tools based on the R system.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Students will become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.</t>
+          <t>Learners will be able to use the Tidyverse to automate tasks efficiently. They will learn how to use best practice techniques in their workflow from data ingestion through to communication of results.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>become familiar with how a plot is built using ggplot and leaflet and ways to build and customise their plots using both packages.</t>
+          <t xml:space="preserve"> Understand the scientific approach to the data analysis workflow and why and how R contributes to the process. ;  Be able to import data into R in different text formats, flat files, excel, SAS, STATA and SPSS files as well as data from the web. ;  Know the concept of tidy data, identify messy features in a data set and tidy it ready for analysis. ;  Use simple exploratory analysis, including visualisation, to understand the data structure and some information it contains and also to detect, be aware of, and possibly correct, data anomalies. ;  Be able to create a basic report  of  data analysis using a R notebook. ;  Work with the Tidyverse packages readr, tidyr, dplyr, stringr, ggplot2, forcats, lubridate, etc. </t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning - Not Available; Face to face - Available</t>
+          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Intermediate</t>
+          <t>Beginner. Familiar with basic R syntax.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_ggplot-leaflet-map-training</t>
+          <t>https://github.com/datasciencecampus/DSCA_DSWR</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Laurie Baker</t>
+          <t>Sonia Mazzi</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Richard Leyshon</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>NULL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Introduction to R</t>
+          <t>Intermediate Python Programming</t>
         </is>
       </c>
       <c r="B6">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10 Hours</t>
+          <t>12 Hours</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Designed for statistical analysis and reporting, R is a powerful tool for data analysis. This course focuses on the application of key data skills, providing opportunities to build confidence, independence, and resilience. This 1 day course will introduce you to the building blocks of R including objects, vectors, and data frames and will examine common data types (e.g. character, factor). During the course we will also cover data manipulation using dplyr and data visualisation using ggplot with examples from the gapminder dataset.</t>
+          <t>This course is delivered through the Jupyter notebook application. It begins with a comprehensive overview of the Pandas library. The two main data structures in this library – the series and dataframe and associated methods are explained with clarifying examples on how to select, filter, aggregate and merge data. Keys tasks like handling null values, applying functions and plotting are also highlighted.  Each section has exercises for participants to attempt to consolidate their learning.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>The aim of this course is to equip you with a toolbox to get started with data in R aand Rstudio and to provide a sound foundation from which to continue your learning beyond the classroom.</t>
+          <t>Participants should become knowledgeable in how to deal with tabular data through using the specialised data structures found in the Pandas library and how to perform key analysis through methods available in this library.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Familiarise themselves with RStudio and R Notebooks, which is what we’ll use to interact with R. ;  Learn about the simple data structures in R: object, vector, and data frame. ;  Explore R's basic data types = integer, character, numeric, etc. ;  Learn to read data into R. ;  Introduction to data wrangling using the tidyverse set of metapackages. ;  Use the tidyverse verbs to explore the gapminder data set which includes statistics for countries around the world including life expectancy, population, and GDP per capita. ;  Learn to merge datasets using left_join. ;  Create meaningful visualisations of the data using ggplot2. ;  Learn where to go for help. </t>
+          <t>Describe specialised data structures - the series and dataframe in the Pandas library; Select, filter, aggregate, merge data in the Pandas dataframe; Execute specific operations to handle null values and apply functions.; Plot data in a dataframe column(s).</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning - Available Soon; Face to face - Available</t>
+          <t>E learning - Available; Self learning - Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>This courses is aimed at complete beginners with no prior programming experience.</t>
+          <t>Completion of introduction to python course. Basic literacy in python code.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Intro-R</t>
+          <t>https://github.com/datasciencecampus/DSCA_intermediate-python</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Laurie Baker</t>
+          <t>Saliha Minhas</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Richard Leyshon, Kaveh Jahanshahi</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -722,63 +722,55 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Introduction to Natural Language Programming with Python</t>
+          <t>Introduction to R</t>
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6 Hours</t>
+          <t>10 Hours</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Natural Language Processing is a sub-field of Artificial Intelligence.
-It is used for processing and analysing large amounts of natural language.
-Some applications include search engines (Google), text classification (spam filters),
-identifying sentiments for a product (sentiment analysis), methods for discovering
-abstract topics in a collection of documents (topic modelling) and machine translation technologies.
-Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics,
-and application of feature engineering techniques to transform textual data into a numerical representation.
-Key techniques such as word embeddings and language modelling are also introduced as well as illustrations
-as to how they can be performed over a dataset.</t>
+          <t>Designed for statistical analysis and reporting, R is a powerful tool for data analysis. This course focuses on the application of key data skills, providing opportunities to build confidence, independence, and resilience. This 1 day course will introduce you to the building blocks of R including objects, vectors, and data frames and will examine common data types (e.g. character, factor). During the course we will also cover data manipulation using dplyr and data visualisation using ggplot with examples from the gapminder dataset.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Participants should gain competancy in using core techniques to handle natural language content to undertake analysis to detect patterns and derive insights for development of applications like mentioned in course summary</t>
+          <t>The aim of this course is to equip you with a toolbox to get started with data in R aand Rstudio and to provide a sound foundation from which to continue your learning beyond the classroom.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.; Produce clusters using the k-means algorithm to uncover patterns in a corpus; Transform text to vectors using approaches delineated.; Produce word embeddings on a corpus; Calculate the probability of a sentence using a language modelling approach</t>
+          <t xml:space="preserve"> Familiarise themselves with RStudio and R Notebooks, which is what we’ll use to interact with R. ;  Learn about the simple data structures in R: object, vector, and data frame. ;  Explore R's basic data types = integer, character, numeric, etc. ;  Learn to read data into R. ;  Introduction to data wrangling using the tidyverse set of metapackages. ;  Use the tidyverse verbs to explore the gapminder data set which includes statistics for countries around the world including life expectancy, population, and GDP per capita. ;  Learn to merge datasets using left_join. ;  Create meaningful visualisations of the data using ggplot2. ;  Learn where to go for help. </t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
+          <t>E learning - Available; Self learning - Available Soon; Face to face - Available</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Competency in using the Python Programming language to perform basic data manipulation is reqiured.</t>
+          <t>This courses is aimed at complete beginners with no prior programming experience.</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_introNLPpython</t>
+          <t>https://github.com/datasciencecampus/DSCA_Intro-R</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Saliha Minhas</t>
+          <t>Laurie Baker</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Kaveh Jahanshahi</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -790,7 +782,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Introduction to Python Programming</t>
+          <t>Introduction to Natural Language Programming with Python</t>
         </is>
       </c>
       <c r="B8">
@@ -798,42 +790,37 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>6 to 8 Hours</t>
+          <t>6 Hours</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>This course is delivered through the Jupyter notebook application.
-It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists,
-dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types
-to compose code with selection and iteration constructs.  To promote modular and readable code the set-up
-and use of functions with parameters are also covered.</t>
+          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language. Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. Concepts covered include cleaning, exploring datasets through methods rooted in Corpus Linguistics, and application of feature engineering techniques to transform textual data into a numerical representation. Key techniques such as word embeddings and language modelling are also introduced as well as illustrations as to how they can be performed over a dataset.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Participants should attain a good understanding of basic data types in Python and associated methods
-and constructs that can be applied to them.</t>
+          <t>Participants should gain competancy in using core techniques to handle natural language content to undertake analysis to detect patterns and derive insights for development of applications like mentioned in course summary</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code</t>
+          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.; Produce clusters using the k-means algorithm to uncover patterns in a corpus; Transform text to vectors using approaches delineated.; Produce word embeddings on a corpus; Calculate the probability of a sentence using a language modelling approach</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning - Available Soon; Face to face - Available</t>
+          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>No previous experience in coding is required though a  basic digital literacy assumed.</t>
+          <t>Competency in using the Python Programming language to perform basic data manipulation is reqiured.</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_intropython</t>
+          <t>https://github.com/datasciencecampus/DSCA_introNLPpython</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -843,8 +830,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Richard Leyshon,
-Kaveh Jahanshahi</t>
+          <t>Kaveh Jahanshahi Jonathon Mellor</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -856,68 +842,67 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Fundemental theories in Machine Learning</t>
+          <t>Introduction to Python Programming</t>
         </is>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8 Hours</t>
+          <t>6 to 8 Hours</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>This course covers the fundemental topics in machine learning and prepare audience for more advanced topics (e.g. image processing, NLP, and deep learning) and practical courses such as training and application of machine learning algorithms in R and Python. The course includes combination of graphical presentation and intuition and essential mathematical notations.</t>
+          <t>This course is delivered through the Jupyter notebook application. It begins with a coverage of fundamental building blocks in Python -  numeric data types, strings, lists, dictionaries, sets - replete with examples. Illustrations are then provided on the use of these data types to compose code with selection and iteration constructs.  To promote modular and readable code the set-up and use of functions with parameters are also covered.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Provide a thorough introduction into probability theory and statistical inference including maximum-likelihood and Bayesian approaches. Introduce supervised learning methods: linear and nonlinear regressions and classification algorithms. Introduce unsupervised learning methods: clustering, and dimensionality reduction. Brief introduction to Directed Graphical Models with a case study/example.</t>
+          <t>Participants should attain a good understanding of basic data types in Python and associated methods and constructs that can be applied to them.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Be able to describe the diffence between frequentist and bayesian statistics; Understand the fundementals of probability theory, bayesian rule and inference, and the characteristics of major probability distributions.; Get a good understanding of major supervised learning algorithms specifically linear in parameter regression, bayesian linear regression, and classification methods.; Get a good understanding of main unsupervised learning algorithms specifically clustering and data dimensionality reduction algorithms.; Get familiar with directed graphical method as a technique of combining supervised and unsupervised learning into one modelling framework; be prepared to build on their current knowledge or take on more advanced courses such as application of machine learning techniques in natural language processing; be prepared to apply their knowledge through formulating machine learning problems and coding using standard libraries (e.g. in R and Python)</t>
+          <t>Describe basic data types in Python; Apply methods to basic data types; Enact selection and iteration over basic data types; Construct functions to compose modular code</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
+          <t>E learning - Available; Self learning - Available Soon; Face to face - Available</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Some basic knowledge in linear algebra and statistics is expected.</t>
+          <t>No previous experience in coding is required though a  basic digital literacy assumed.</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_ML_theory</t>
+          <t>https://github.com/datasciencecampus/DSCA_intropython</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Kaveh Jahanshahi</t>
+          <t>Saliha Minhas</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Laurie Baker 
-Isabela Breton</t>
+          <t>Richard Leyshon, Kaveh Jahanshahi</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>MIT License</t>
+          <t>NULL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Natural Language Processing with R</t>
+          <t>Fundemental theories in Machine Learning</t>
         </is>
       </c>
       <c r="B10">
@@ -930,22 +915,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Natural Language Processing is a sub-field of Artificial Intelligence.
-It is used for processing and analysing large amounts of natural language (texts).
-Some applications include search engines (Google), text classification (spam filters),
-identifying sentiments for a product (sentiment analysis), methods for discovering
-abstract topics in a collection of documents (topic modelling) and machine translation technologies.
-In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
+          <t>This course covers the fundemental topics in machine learning and prepare audience for more advanced topics (e.g. image processing, NLP, and deep learning) and practical courses such as training and application of machine learning algorithms in R and Python. The course includes combination of graphical presentation and intuition and essential mathematical notations.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
+          <t>Provide a thorough introduction into probability theory and statistical inference including maximum-likelihood and Bayesian approaches. Introduce supervised learning methods: linear and nonlinear regressions and classification algorithms. Introduce unsupervised learning methods: clustering, and dimensionality reduction. Brief introduction to Directed Graphical Models with a case study/example.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
+          <t>Be able to describe the diffence between frequentist and bayesian statistics; Understand the fundementals of probability theory, bayesian rule and inference, and the characteristics of major probability distributions.; Get a good understanding of major supervised learning algorithms specifically linear in parameter regression, bayesian linear regression, and classification methods.; Get a good understanding of main unsupervised learning algorithms specifically clustering and data dimensionality reduction algorithms.; Get familiar with directed graphical method as a technique of combining supervised and unsupervised learning into one modelling framework; be prepared to build on their current knowledge or take on more advanced courses such as application of machine learning techniques in natural language processing; be prepared to apply their knowledge through formulating machine learning problems and coding using standard libraries (e.g. in R and Python)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -955,34 +935,34 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
+          <t>Some basic knowledge in linear algebra and statistics is expected.</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
+          <t>https://github.com/datasciencecampus/DSCA_ML_theory</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Sonia Mazzi</t>
+          <t>Kaveh Jahanshahi</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Kaveh Jahanshahi</t>
+          <t>Laurie Baker  Isabela Breton</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>MIT License</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Introduction to Reproducibility</t>
+          <t>Natural Language Processing with R</t>
         </is>
       </c>
       <c r="B11">
@@ -990,48 +970,47 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6 Hours</t>
+          <t>8 Hours</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Introduction to reproducibility. What is a reproducible analytical pipeline (RAP), writing "good code" and creating a reproducible report.</t>
+          <t>Natural Language Processing is a sub-field of Artificial Intelligence. It is used for processing and analysing large amounts of natural language (texts). Some applications include search engines (Google), text classification (spam filters), identifying sentiments for a product (sentiment analysis), methods for discovering abstract topics in a collection of documents (topic modelling) and machine translation technologies. In this course you learn about exploratory analysis of text data, introduced to sentiment analysis of texts using sentiment lexicons and the concept of topic modelling (package topicmodels).</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Participants should gain an awareness of the importance of reproducibility in their work. Learners will also gain experience of linting code in Python and using parameterised reports in R markdown.</t>
+          <t>At the end of this course you should be able to set text data into a form that can be used for analysis, carry out cleaning of text data, exploratory analysis of text data, use meta-data to produce interesting visual displays depicting features of the text data, carry out sentiment analysis using  sentiment lexicons and discover topics in a corpus.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>represent pipelines and identify opportunities to automate; consider adherance to a programming style guide; use linting software to standardise Python scripts; use parameterised R markdown reports to improve the efficiency of report production.</t>
+          <t>Describe the main components of language structure; Perform pre-processing (cleaning) operations on text.; Apply methods from Corpus Linguistics to garner greater insights on a corpus.; Produce word-clouds, bar charts and other basic visualisations on variables of interest.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
+          <t>E learning - Available; Self learning -  Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Basic familiarity with Python and R programming is assumed.</t>
+          <t>Competency in using the R Programming language to perform basic data manipulation is reqiured. For that refer to Intro to R (https://github.com/datasciencecampus/DSCA_Intro-R)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_reproducibility</t>
+          <t>https://github.com/datasciencecampus/DSCA_NLPWR</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Laurie L. Baker
-Richard Leyshon</t>
+          <t>Sonia Mazzi</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Kaveh Jahanshahi</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1043,7 +1022,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Statistics for Data Science</t>
+          <t>Introduction to Reproducibility</t>
         </is>
       </c>
       <c r="B12">
@@ -1051,42 +1030,42 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>18 Hours</t>
+          <t>6 Hours</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>This course introduces the basics of carrying out a statistical analysis in Python. It covers exploratory data analysis, constructing and interpreting linear and generalized linear models, and introduces Bayesian modelling.</t>
+          <t>Introduction to reproducibility. What is a reproducible analytical pipeline (RAP), writing "good code" and creating a reproducible report.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
+          <t>Participants should gain an awareness of the importance of reproducibility in their work. Learners will also gain experience of linting code in Python and using parameterised reports in R markdown.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
+          <t>represent pipelines and identify opportunities to automate; consider adherance to a programming style guide; use linting software to standardise Python scripts; use parameterised R markdown reports to improve the efficiency of report production.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
+          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
+          <t>Basic familiarity with Python and R programming is assumed.</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
+          <t>https://github.com/datasciencecampus/DSCA_reproducibility</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Laurie Baker, Dan Lewis</t>
+          <t>Laurie L. Baker Richard Leyshon</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1103,7 +1082,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Version Control with Git: Github</t>
+          <t>Statistics for Data Science</t>
         </is>
       </c>
       <c r="B13">
@@ -1111,42 +1090,42 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4 Hours</t>
+          <t>18 Hours</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Publications that make the used code available have generally higher impact than publications where code is not available. One important tool for code quality and code sharing is a version control system (VCS). A version control system is a tool that manages changes made to the files and directories in a project. Git, together with GitHub, is one such VCS tool.</t>
+          <t>This course introduces the basics of carrying out a statistical analysis in Python. It covers exploratory data analysis, constructing and interpreting linear and generalized linear models, and introduces Bayesian modelling.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
+          <t>By the end of the course students will be comfortable implementing and interpreting linear models and generalized linear model in Python and be familiar with the concepts of Bayesian modelling.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
+          <t>What is tidy data? What is a variable, value, and observation? Several python commands to explore the structure of the data What is the difference between a continuous and categorical variable? What is variation and covariation? ; What is a variable, value, and observation?; Several python commands to explore the structure of the data; What is the difference between a continuous and categorical variable?; What is variation and covariation?; Where Exploratory Data Analysis fits within data analysis? How to use plots to explore variation in continuous variable and categorical variables How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable. ; How to use plots to explore variation in continuous variable and categorical variables; How to use plots to explore covariation between two categorical variables, two continuous variables or a categorical and continuous variable.;  Model Basics What is a model family and fitted model? What is the difference between a response and an explanatory variable? ; What is a model family and fitted model?; What is the difference between a response and an explanatory variable?;  Model Construction How to construct a linear model in python? What are the slope and intercept in a linear model? Picking out key information from the model table How to extract specific parameters from the model object. ; How to construct a linear model in python?; What are the slope and intercept in a linear model?; Picking out key information from the model table; How to extract specific parameters from the model object.;  Assessing Model Fit How to inspect model residuals to assess model fit? How to pick out key information from the table from a fitted model. How to use Adjusted R-squared and AIC to compare models. ; How to inspect model residuals to assess model fit?; How to pick out key information from the table from a fitted model.; How to use Adjusted R-squared and AIC to compare models.;  What is probability? ;  What is a random variable? ;  What a probability distribution is and how it differs for continuous vs. discrete random variables? ;  Be familiar with several common probability distributions used to model variation in the response variable Binomial Normal Poisson Negative Binomial ; Binomial; Normal; Poisson; Negative Binomial;  How to implement a generalized linear model in python. ; What is Baye's rule and how it is used in Bayesian statistics?; How Bayesian and Frequentist schools of thought differ?; How to implement a simple Bayesian linear model in python.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
+          <t>E learning - Not Available; Self learning - Available; Face to face - Available</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Intermediate / Advanced</t>
+          <t>Participants should be familiar with Python but do not need any prior statistical training.</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
+          <t>https://github.com/datasciencecampus/DSCA_Stats4DS</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Sonia Mazzi</t>
+          <t>Laurie Baker, Dan Lewis</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1163,7 +1142,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Version controlled RStudio projects</t>
+          <t>Version Control with Git: Github</t>
         </is>
       </c>
       <c r="B14">
@@ -1176,45 +1155,105 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>Publications that make the used code available have generally higher impact than publications where code is not available. One important tool for code quality and code sharing is a version control system (VCS). A version control system is a tool that manages changes made to the files and directories in a project. Git, together with GitHub, is one such VCS tool.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Learners will be able to use Github to create, manage and collaborate on projects.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Use Git in their workflow; Use a selection of important Git functions to manage their workflow; Make adjustments to repositories with version control; Unify different versions of the same document</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Intermediate / Advanced</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>https://github.com/datasciencecampus/DSCA_Version-control-with-Git-Github</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Sonia Mazzi</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Version controlled RStudio projects</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4 Hours</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>RStudio has the ability to use version control for R projects using a very easy to use graphical interface. In this course we will introduce how R Studio has integrated Git version control into its interface. This allows developers to efficiently track changes in their code over time and effectively collaborate with a team of programmers. This course explains how to use the Git workflow to revise and track changes to an r markdown document, ultimately publishing your own version to web.</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Learners will be able to use R Studio's integrated Git features to improve their ability to track changes and collaborate in their code.</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Learn how to use the Git workflow to improve your version control &amp; collaboration; Manage the Git workflow right from the R Studio IDE</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>E learning - Not Available; Self learning - Not Available; Face to face - Available</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Intermediate R user.</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>https://github.com/datasciencecampus/DSCA_Version-controlled-RStudio-projects</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Sonia Mazzi</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>

</xml_diff>